<commit_message>
AP llm-transform Part 2
</commit_message>
<xml_diff>
--- a/script/result_llm_tranform/ardupilot_docs/ap_acro-mode/result.xlsx
+++ b/script/result_llm_tranform/ardupilot_docs/ap_acro-mode/result.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12300"/>
+    <workbookView windowWidth="27948" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="mtl" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="197">
   <si>
     <t>index</t>
   </si>
@@ -200,6 +200,9 @@
     <t>B represents body frame controller, R represents rotation, P' represents new pitch angle, and R' represents new roll angle. The formula states that globally, when B and R occur, in the next state (X) the angles will have changed (P' and R'). This captures the immediate effect of rotation in Acro mode.</t>
   </si>
   <si>
+    <t>{'sentence': 'Stick inputs are interpreted in the "body frame" (as opposed to Sport mode in which they are "earth frame").', 'formula': 'G(B ∧ ¬E)', 'explanation': 'Here, B represents stick inputs being interpreted in the body frame, and E represents stick inputs being interpreted in the earth frame. The formula states that globally, stick inputs are interpreted in the body frame and not in the earth frame.'}</t>
+  </si>
+  <si>
     <t>state transition pre-requirement</t>
   </si>
   <si>
@@ -218,6 +221,9 @@
     <t>{'sentence': 'While Acro mode does not necessarily require GPS, switching to RTL in case of emergency does.', 'formula': 'G(¬A → ¬G) ∧ (E → G)', 'explanation': 'Here, A represents Acro mode, G represents GPS, E represents emergency, and RTL represents Return To Launch. The formula states that globally, Acro mode does not require GPS, but in case of emergency, switching to RTL requires GPS.'}</t>
   </si>
   <si>
+    <t>{'sentence': 'Stick inputs are interpreted in the "body frame" (as opposed to Sport mode in which they are "earth frame").', 'formula': 'G(A → B) ∧ G(¬A → E)', 'explanation': 'This formula states that globally (G), when in Acro mode (A), stick inputs are in body frame (B), and when not in Acro mode (¬A), inputs are in earth frame (E). This distinguishes between the two modes of interpretation.'}</t>
+  </si>
+  <si>
     <t>40-41</t>
   </si>
   <si>
@@ -506,13 +512,19 @@
     <t>D represents the default setting, and R represents the 200deg/sec rotation rate. This formula expresses the persistent effect of the default setting on the rotation rate.</t>
   </si>
   <si>
-    <t>{'sentence': 'The default, 4.5, will command a 200deg/sec rotation rate.', 'formula': 'R = 200', 'explanation': 'Here, R represents the rotation rate. The formula states that the default value of 4.5 corresponds to a rotation rate of 200 degrees per second.'}</t>
-  </si>
-  <si>
-    <t>{'sentence': 'The default, 4.5, will command a 200deg/sec rotation rate.', 'formula': 'G(DEFAULT → ROTATION_RATE_200)', 'explanation': 'The predicate DEFAULT indicates the default setting of 4.5, and ROTATION_RATE_200 represents achieving a 200deg/sec rotation. The formula asserts that whenever the default is set, this rotation rate is commanded globally.'}</t>
-  </si>
-  <si>
-    <t>{'sentence': 'The default, 4.5, will command a 200deg/sec rotation rate.', 'formula': 'G((D ∧ X(R)) → S)', 'explanation': "D represents the default setting of 4.5, R represents ACRO_RP_RATE being set, and S represents a 200deg/sec rotation rate. The 'Next' operator X captures the immediate effect of setting the rate."}</t>
+    <t>{'sentence': 'The default, 4.5, will command a 200deg/sec rotation rate.', 'formula': 'R = 200', 'explanation': 'Here, R represents the rotation rate. The formula states that the default value of 4.5 corresponds to a rotation rate of 200 degrees per second.'}
+{'sentence': '1.ACRO_RP_RATE controls the rotation rate for the roll and pitch axis.', 'formula': 'R', 'explanation': 'This sentence simply states that the ACRO_RP_RATE parameter controls the rotation rate, which is represented by the predicate R.'}
+{'sentence': 'Higher values lead to higher rotation rates, lower to slower rotation rates.', 'formula': 'G((V &gt; 4.5) → (R &gt; 200)) ∧ G((V &lt; 4.5) → (R &lt; 200))', 'explanation': 'Here, V represents the value of the ACRO_RP_RATE parameter, and R represents the rotation rate. The formula ensures that higher values of the parameter always lead to higher rotation rates, and lower values always lead to slower rotation rates.'}</t>
+  </si>
+  <si>
+    <t>{'sentence': 'The default, 4.5, will command a 200deg/sec rotation rate.', 'formula': 'G(DEFAULT → ROTATION_RATE_200)', 'explanation': 'The predicate DEFAULT indicates the default setting of 4.5, and ROTATION_RATE_200 represents achieving a 200deg/sec rotation. The formula asserts that whenever the default is set, this rotation rate is commanded globally.'}
+{'sentence': "Let's say you have a highly nimble quadcopter and you have your ACRO_RP_RATE parameter set to 9, which translates to a roll request of ~400deg/sec.", 'formula': 'G(N ∧ R₉)', 'explanation': 'N represents having a nimble quadcopter, and R₉ represents setting ACRO_RP_RATE to 9, leading to a roll rate of ~400deg/sec.'}</t>
+  </si>
+  <si>
+    <t>{'sentence': 'The default, 4.5, will command a 200deg/sec rotation rate.', 'formula': 'G((D ∧ X(R)) → S)', 'explanation': "D represents the default setting of 4.5, R represents ACRO_RP_RATE being set, and S represents a 200deg/sec rotation rate. The 'Next' operator X captures the immediate effect of setting the rate."}
+{'sentence': '1.ACRO_RP_RATE controls the rotation rate for the roll and pitch axis.', 'formula': 'G(R ↔ (X ∧ Y))', 'explanation': 'R represents ACRO_RP_RATE, X represents the roll axis rotation rate, and Y represents the pitch axis rotation rate. This formula captures the control relationship between ACRO_RP_RATE and both axes.'}
+{'sentence': "Let's say you have a highly nimble quadcopter and you have your ACRO_RP_RATE parameter set to 9, which translates to a roll request of ~400deg/sec.", 'formula': 'G(N ∧ A → F(R))', 'explanation': 'N represents a nimble quadcopter, A represents ACRO_RP_RATE set to 9, and R represents a roll request of ~400deg/sec. The formula states that globally, when we have a nimble quadcopter and the ACRO_RP_RATE is set to 9, it will eventually lead to a high roll request.'}
+{'sentence': 'Higher values lead to higher rotation rates, lower to slower rotation rates.', 'formula': 'G((H → F(R)) ∧ (L → F(S)))', 'explanation': 'This formula states that globally, if we have higher values (H), it will eventually lead to higher rotation rates (R), and if we have lower values (L), it will eventually lead to slower rotation rates (S). The use of G ensures this relationship holds at all times.'}</t>
   </si>
   <si>
     <t>102-103</t>
@@ -536,27 +548,12 @@
     <t>{'sentence': 'The default, 4.5, like roll and pitch, will command a 200deg/sec rotation rate.', 'formula': 'G(D → X(R))', 'explanation': 'D represents the default setting of 4.5, and R represents the 200deg/sec rotation rate. The formula states that globally, when D is true, in the next state, R will be true, representing the command of the specific rotation rate.'}</t>
   </si>
   <si>
-    <t>{'sentence': 'Stick inputs are interpreted in the "body frame" (as opposed to Sport mode in which they are "earth frame").', 'formula': 'G(B ∧ ¬E)', 'explanation': 'Here, B represents stick inputs being interpreted in the body frame, and E represents stick inputs being interpreted in the earth frame. The formula states that globally, stick inputs are interpreted in the body frame and not in the earth frame.'}</t>
-  </si>
-  <si>
-    <t>{'sentence': "Let's say you have a highly nimble quadcopter and you have your ACRO_RP_RATE parameter set to 9, which translates to a roll request of ~400deg/sec.", 'formula': 'G(N ∧ R₉)', 'explanation': 'N represents having a nimble quadcopter, and R₉ represents setting ACRO_RP_RATE to 9, leading to a roll rate of ~400deg/sec.'}</t>
-  </si>
-  <si>
     <t>{'sentence': 'Acro mode uses the RC sticks to control the angular velocity of the copter in each axis.', 'formula': 'G(A → (R ∧ V))', 'explanation': 'This formula states that globally (G), when Acro mode is active (A), it implies (→) that RC stick input (R) and angular velocity control (V) are both true. This captures the continuous nature of the control in Acro mode.'}</t>
   </si>
   <si>
-    <t>{'sentence': '1.ACRO_RP_RATE controls the rotation rate for the roll and pitch axis.', 'formula': 'R', 'explanation': 'This sentence simply states that the ACRO_RP_RATE parameter controls the rotation rate, which is represented by the predicate R.'}</t>
-  </si>
-  <si>
     <t>{'sentence': 'The Virtual Flybar will add decay term to the attitude controller to bleed off accumulated differences between the current attitude and accumulated commanded attitude, if the copter has not quickly obtained it, such as when sitting on the ground but stick inputs are being given.', 'formula': 'G((¬Q ∧ G) → D)', 'explanation': 'Q represents the copter quickly obtaining the commanded attitude, G indicates sitting on the ground with stick inputs, and D represents the Virtual Flybar adding a decay term.'}</t>
   </si>
   <si>
-    <t>{'sentence': 'Stick inputs are interpreted in the "body frame" (as opposed to Sport mode in which they are "earth frame").', 'formula': 'G(A → B) ∧ G(¬A → E)', 'explanation': 'This formula states that globally (G), when in Acro mode (A), stick inputs are in body frame (B), and when not in Acro mode (¬A), inputs are in earth frame (E). This distinguishes between the two modes of interpretation.'}</t>
-  </si>
-  <si>
-    <t>{'sentence': 'Higher values lead to higher rotation rates, lower to slower rotation rates.', 'formula': 'G((V &gt; 4.5) → (R &gt; 200)) ∧ G((V &lt; 4.5) → (R &lt; 200))', 'explanation': 'Here, V represents the value of the ACRO_RP_RATE parameter, and R represents the rotation rate. The formula ensures that higher values of the parameter always lead to higher rotation rates, and lower values always lead to slower rotation rates.'}</t>
-  </si>
-  <si>
     <t>{'sentence': 'This value can be increased to improve attitude control when the throttle is cut for better Airmode handling, however a stable tune is essential before it can be increased.', 'formula': 'G((THROTTLE_CUT ∧ STABLE_TUNE) → F(INCREASE_VALUE ∧ IMPROVED_CONTROL))', 'explanation': 'This formula states that globally, if the throttle is cut and a stable tune is achieved, eventually the value can be increased leading to improved attitude control.'}</t>
   </si>
   <si>
@@ -569,18 +566,12 @@
     <t>{'sentence': 'Raising the INS_GYRO_FILTER cutoff frequency and retuning may allow better responsiveness, but appropriate harmonic notch filtering to prevent noise impacts must be setup prior to retuning.', 'formula': 'G((NOTCH_FILTER_SETUP ∧ RETUNING) → F(BETTER_RESPONSIVENESS))', 'explanation': 'This formula indicates that globally, setting up the notch filter and retuning will eventually allow for better responsiveness. The setup is a prerequisite to retuning.'}</t>
   </si>
   <si>
-    <t>{'sentence': '1.ACRO_RP_RATE controls the rotation rate for the roll and pitch axis.', 'formula': 'G(R ↔ (X ∧ Y))', 'explanation': 'R represents ACRO_RP_RATE, X represents the roll axis rotation rate, and Y represents the pitch axis rotation rate. This formula captures the control relationship between ACRO_RP_RATE and both axes.'}</t>
-  </si>
-  <si>
     <t>{'sentence': '3.ACRO_RP_EXPO and ACRO_Y_EXPO are an amount of Exponential to apply to the pilots stick inputs that only applies to ACRO mode.', 'formula': 'G((ARE ∧ AYE) → (E ∧ AM))', 'explanation': 'Here, ARE and AYE represent the ACRO_RP_EXPO and ACRO_Y_EXPO being applied respectively, E represents the exponential being applied, and AM represents the ACRO mode being active. The formula states that globally, whenever both ACRO_RP_EXPO and ACRO_Y_EXPO are applied, they apply an exponential to the pilots stick inputs only in ACRO mode.'}</t>
   </si>
   <si>
     <t>{'sentence': 'Sentence not found.', 'formula': '', 'explanation': 'No MTL formula is provided as the sentence is not found.'}</t>
   </si>
   <si>
-    <t>{'sentence': 'Higher values lead to higher rotation rates, lower to slower rotation rates.', 'formula': 'G((H → F(R)) ∧ (L → F(S)))', 'explanation': 'This formula states that globally, if we have higher values (H), it will eventually lead to higher rotation rates (R), and if we have lower values (L), it will eventually lead to slower rotation rates (S). The use of G ensures this relationship holds at all times.'}</t>
-  </si>
-  <si>
     <t>{'sentence': '1.ATC_ACCEL_R_MAX and ATC_ACCEL_P_MAX: Maximum acceleration in roll/pitch axis measured in Centi-degres/sec/sec.', 'formula': 'G((ARM ∧ APM) → (M ∧ (R ∨ P)))', 'explanation': 'Here, ARM and APM represent the ATC_ACCEL_R_MAX and ATC_ACCEL_P_MAX being applied respectively, M represents the maximum acceleration being measured, and R and P represent the roll and pitch axes respectively. The formula states that globally, whenever both ATC_ACCEL_R_MAX and ATC_ACCEL_P_MAX are applied, they measure the maximum acceleration in either roll or pitch axis.'}</t>
   </si>
   <si>
@@ -606,9 +597,6 @@
   </si>
   <si>
     <t>{'sentence': '1.ATC_ACCEL_R_MAX and ATC_ACCEL_P_MAX: Maximum acceleration in roll/pitch axis measured in Centi-degres/sec/sec.', 'formula': 'G((R → M) ∧ (P → M))', 'explanation': 'R represents ATC_ACCEL_R_MAX, P represents ATC_ACCEL_P_MAX, and M represents the maximum acceleration. This formula states that globally, both R and P imply M, capturing the definition of these parameters as maximum accelerations.'}</t>
-  </si>
-  <si>
-    <t>{'sentence': "Let's say you have a highly nimble quadcopter and you have your ACRO_RP_RATE parameter set to 9, which translates to a roll request of ~400deg/sec.", 'formula': 'G(N ∧ A → F(R))', 'explanation': 'N represents a nimble quadcopter, A represents ACRO_RP_RATE set to 9, and R represents a roll request of ~400deg/sec. The formula states that globally, when we have a nimble quadcopter and the ACRO_RP_RATE is set to 9, it will eventually lead to a high roll request.'}</t>
   </si>
   <si>
     <t>{'sentence': 'The copter is not physically capable of going from 0deg/sec to 400deg/sec without a brief moment of acceleration.', 'formula': 'G(¬(Z ∧ X(H)))', 'explanation': "Z represents 0deg/sec, and H represents 400deg/sec. This formula states that globally, it's not true that we can have 0deg/sec and immediately in the next state have 400deg/sec, capturing the physical limitation of the copter."}</t>
@@ -1625,15 +1613,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:L53"/>
+  <dimension ref="A1:L54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
+      <selection pane="bottomLeft" activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="25.8" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="7.22222222222222" customWidth="1"/>
     <col min="2" max="2" width="25.1111111111111" customWidth="1"/>
@@ -1649,7 +1637,7 @@
     <col min="12" max="12" width="4.88888888888889" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" ht="28.8" spans="1:12">
+    <row r="1" s="1" customFormat="1" customHeight="1" spans="1:12">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1687,7 +1675,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" s="1" customFormat="1" ht="409.5" spans="1:12">
+    <row r="2" s="1" customFormat="1" customHeight="1" spans="1:12">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1725,7 +1713,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" s="1" customFormat="1" ht="409.5" spans="1:12">
+    <row r="3" s="1" customFormat="1" customHeight="1" spans="1:12">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1753,15 +1741,17 @@
       <c r="I3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J3" s="1"/>
+      <c r="J3" s="1">
+        <v>1</v>
+      </c>
       <c r="K3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="L3" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" s="1" customFormat="1" ht="115.2" spans="1:12">
+      <c r="L3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" s="1" customFormat="1" customHeight="1" spans="1:12">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1799,7 +1789,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" s="1" customFormat="1" ht="409.5" spans="1:12">
+    <row r="5" s="1" customFormat="1" customHeight="1" spans="1:12">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1821,8 +1811,8 @@
       <c r="G5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>7</v>
+      <c r="H5" s="1">
+        <v>1</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>7</v>
@@ -1833,11 +1823,11 @@
       <c r="K5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="L5" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" s="1" customFormat="1" ht="409.5" spans="1:12">
+      <c r="L5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" s="1" customFormat="1" customHeight="1" spans="1:12">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1859,23 +1849,23 @@
       <c r="G6" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>7</v>
+      <c r="H6" s="1">
+        <v>1</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="J6" s="1" t="s">
-        <v>7</v>
+      <c r="J6" s="1">
+        <v>1</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="L6" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" s="1" customFormat="1" ht="86.4" spans="1:12">
+      <c r="L6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" s="1" customFormat="1" customHeight="1" spans="1:12">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1913,7 +1903,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" s="1" customFormat="1" ht="409.5" spans="1:12">
+    <row r="8" s="1" customFormat="1" customHeight="1" spans="1:12">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1935,8 +1925,8 @@
       <c r="G8" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H8" s="1" t="s">
-        <v>7</v>
+      <c r="H8" s="1">
+        <v>1</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>7</v>
@@ -1951,7 +1941,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" s="1" customFormat="1" ht="100.8" spans="1:12">
+    <row r="9" s="1" customFormat="1" customHeight="1" spans="1:12">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1989,7 +1979,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" s="1" customFormat="1" ht="100.8" spans="1:12">
+    <row r="10" s="1" customFormat="1" customHeight="1" spans="1:12">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -2009,10 +1999,10 @@
         <v>56</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>7</v>
+        <v>57</v>
+      </c>
+      <c r="H10" s="1">
+        <v>1</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>7</v>
@@ -2027,30 +2017,30 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" s="1" customFormat="1" ht="409.5" spans="1:12">
+    <row r="11" s="1" customFormat="1" customHeight="1" spans="1:12">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>7</v>
+        <v>63</v>
+      </c>
+      <c r="H11" s="1">
+        <v>1</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>7</v>
@@ -2059,51 +2049,51 @@
         <v>7</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" s="1" customFormat="1" ht="409.5" spans="1:12">
+        <v>64</v>
+      </c>
+      <c r="L11" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" s="1" customFormat="1" customHeight="1" spans="1:12">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>7</v>
+        <v>69</v>
+      </c>
+      <c r="H12" s="1">
+        <v>1</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>7</v>
+        <v>70</v>
+      </c>
+      <c r="J12" s="1">
+        <v>0</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" s="1" customFormat="1" ht="409.5" spans="1:12">
+        <v>71</v>
+      </c>
+      <c r="L12" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" s="1" customFormat="1" customHeight="1" spans="1:12">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -2111,37 +2101,37 @@
         <v>43</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>7</v>
+        <v>76</v>
+      </c>
+      <c r="H13" s="1">
+        <v>1</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>7</v>
+        <v>77</v>
+      </c>
+      <c r="J13" s="1">
+        <v>1</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" s="1" customFormat="1" ht="316.8" spans="1:12">
+        <v>78</v>
+      </c>
+      <c r="L13" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" s="1" customFormat="1" customHeight="1" spans="1:12">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -2149,22 +2139,22 @@
         <v>10</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>7</v>
+        <v>83</v>
+      </c>
+      <c r="H14" s="1">
+        <v>1</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>7</v>
@@ -2179,7 +2169,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" s="1" customFormat="1" ht="409.5" spans="1:12">
+    <row r="15" s="1" customFormat="1" customHeight="1" spans="1:12">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -2187,22 +2177,22 @@
         <v>10</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>7</v>
+        <v>88</v>
+      </c>
+      <c r="H15" s="1">
+        <v>1</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>7</v>
@@ -2217,7 +2207,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" s="1" customFormat="1" ht="288" spans="1:12">
+    <row r="16" s="1" customFormat="1" customHeight="1" spans="1:12">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -2225,22 +2215,22 @@
         <v>10</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>7</v>
+        <v>93</v>
+      </c>
+      <c r="H16" s="1">
+        <v>0</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>7</v>
@@ -2249,13 +2239,13 @@
         <v>7</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="L16" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" s="1" customFormat="1" ht="409.5" spans="1:12">
+        <v>94</v>
+      </c>
+      <c r="L16" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" s="1" customFormat="1" customHeight="1" spans="1:12">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -2263,37 +2253,37 @@
         <v>10</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>7</v>
+        <v>99</v>
+      </c>
+      <c r="H17" s="1">
+        <v>1</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>7</v>
+        <v>100</v>
+      </c>
+      <c r="J17" s="1">
+        <v>1</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="L17" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" s="1" customFormat="1" ht="72" spans="1:12">
+        <v>101</v>
+      </c>
+      <c r="L17" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" s="1" customFormat="1" customHeight="1" spans="1:12">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -2301,16 +2291,16 @@
         <v>10</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>7</v>
@@ -2331,7 +2321,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" s="1" customFormat="1" ht="72" spans="1:12">
+    <row r="19" s="1" customFormat="1" customHeight="1" spans="1:12">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -2339,16 +2329,16 @@
         <v>10</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>7</v>
@@ -2369,7 +2359,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" s="1" customFormat="1" ht="316.8" spans="1:12">
+    <row r="20" s="1" customFormat="1" customHeight="1" spans="1:12">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -2377,22 +2367,22 @@
         <v>10</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>7</v>
+        <v>114</v>
+      </c>
+      <c r="H20" s="1">
+        <v>1</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>7</v>
@@ -2401,13 +2391,13 @@
         <v>7</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="L20" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" s="1" customFormat="1" ht="409.5" spans="1:12">
+        <v>115</v>
+      </c>
+      <c r="L20" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" s="1" customFormat="1" customHeight="1" spans="1:12">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -2415,37 +2405,37 @@
         <v>43</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>7</v>
+        <v>120</v>
+      </c>
+      <c r="H21" s="1">
+        <v>1</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>7</v>
+        <v>121</v>
+      </c>
+      <c r="J21" s="1">
+        <v>0</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="L21" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" s="1" customFormat="1" ht="360" spans="1:12">
+        <v>122</v>
+      </c>
+      <c r="L21" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" s="1" customFormat="1" customHeight="1" spans="1:12">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -2453,16 +2443,16 @@
         <v>43</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>7</v>
@@ -2477,13 +2467,13 @@
         <v>7</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="L22" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" s="1" customFormat="1" ht="409.5" spans="1:12">
+        <v>127</v>
+      </c>
+      <c r="L22" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" s="1" customFormat="1" customHeight="1" spans="1:12">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -2491,16 +2481,16 @@
         <v>10</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>7</v>
@@ -2509,19 +2499,19 @@
         <v>7</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>7</v>
+        <v>132</v>
+      </c>
+      <c r="J23" s="1">
+        <v>1</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="L23" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="24" s="1" customFormat="1" ht="302.4" spans="1:12">
+        <v>133</v>
+      </c>
+      <c r="L23" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" s="1" customFormat="1" customHeight="1" spans="1:12">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -2529,16 +2519,16 @@
         <v>10</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>7</v>
@@ -2553,13 +2543,13 @@
         <v>7</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="L24" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" s="1" customFormat="1" ht="409.5" spans="1:12">
+        <v>138</v>
+      </c>
+      <c r="L24" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" s="1" customFormat="1" customHeight="1" spans="1:12">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -2567,37 +2557,37 @@
         <v>10</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>7</v>
+        <v>143</v>
+      </c>
+      <c r="H25" s="1">
+        <v>1</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>7</v>
+        <v>144</v>
+      </c>
+      <c r="J25" s="1">
+        <v>1</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="L25" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" s="1" customFormat="1" ht="345.6" spans="1:12">
+        <v>145</v>
+      </c>
+      <c r="L25" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" s="1" customFormat="1" customHeight="1" spans="1:12">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -2605,16 +2595,16 @@
         <v>10</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>7</v>
@@ -2629,13 +2619,13 @@
         <v>7</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="L26" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="27" s="1" customFormat="1" ht="403.2" spans="1:12">
+        <v>150</v>
+      </c>
+      <c r="L26" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" s="1" customFormat="1" customHeight="1" spans="1:12">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -2643,22 +2633,22 @@
         <v>43</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>7</v>
+        <v>155</v>
+      </c>
+      <c r="H27" s="1">
+        <v>1</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>7</v>
@@ -2667,13 +2657,13 @@
         <v>7</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="L27" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="28" s="1" customFormat="1" ht="360" spans="1:12">
+        <v>156</v>
+      </c>
+      <c r="L27" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" s="1" customFormat="1" customHeight="1" spans="1:12">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -2681,37 +2671,37 @@
         <v>10</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>7</v>
+        <v>161</v>
+      </c>
+      <c r="H28" s="1">
+        <v>1</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="J28" s="1" t="s">
-        <v>7</v>
+        <v>162</v>
+      </c>
+      <c r="J28" s="1">
+        <v>1</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="L28" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29" s="1" customFormat="1" ht="409.5" spans="1:12">
+        <v>163</v>
+      </c>
+      <c r="L28" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" s="1" customFormat="1" customHeight="1" spans="1:12">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -2719,37 +2709,37 @@
         <v>10</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>7</v>
+        <v>168</v>
+      </c>
+      <c r="H29" s="1">
+        <v>1</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="J29" s="1" t="s">
-        <v>7</v>
+        <v>169</v>
+      </c>
+      <c r="J29" s="1">
+        <v>1</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="L29" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="30" s="1" customFormat="1" spans="1:12">
+        <v>170</v>
+      </c>
+      <c r="L29" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" s="1" customFormat="1" customHeight="1" spans="1:12">
       <c r="A30" s="1" t="s">
         <v>7</v>
       </c>
@@ -2787,7 +2777,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" s="1" customFormat="1" spans="1:12">
+    <row r="31" s="1" customFormat="1" customHeight="1" spans="1:12">
       <c r="A31" s="1" t="s">
         <v>7</v>
       </c>
@@ -2825,7 +2815,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" s="1" customFormat="1" spans="1:12">
+    <row r="32" s="1" customFormat="1" customHeight="1" spans="1:12">
       <c r="A32" s="1" t="s">
         <v>7</v>
       </c>
@@ -2863,7 +2853,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" s="1" customFormat="1" ht="409.5" spans="1:12">
+    <row r="33" s="1" customFormat="1" customHeight="1" spans="1:12">
       <c r="A33" s="1" t="s">
         <v>7</v>
       </c>
@@ -2882,26 +2872,22 @@
       <c r="F33" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G33" s="1" t="s">
-        <v>169</v>
-      </c>
+      <c r="G33" s="1"/>
       <c r="H33" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I33" s="1" t="s">
-        <v>170</v>
-      </c>
+      <c r="I33" s="1"/>
       <c r="J33" s="1" t="s">
         <v>7</v>
       </c>
       <c r="K33" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="L33" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="34" s="1" customFormat="1" ht="374.4" spans="1:12">
+      <c r="L33" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" s="1" customFormat="1" customHeight="1" spans="1:12">
       <c r="A34" s="1" t="s">
         <v>7</v>
       </c>
@@ -2920,717 +2906,735 @@
       <c r="F34" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G34" s="1" t="s">
+      <c r="G34" s="1"/>
+      <c r="H34" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I34" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="H34" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I34" s="1" t="s">
+      <c r="J34" s="1">
+        <v>0</v>
+      </c>
+      <c r="K34" s="1"/>
+      <c r="L34" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" s="1" customFormat="1" customHeight="1" spans="1:12">
+      <c r="A35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I35" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="J34" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K34" s="1" t="s">
+      <c r="J35" s="1">
+        <v>0</v>
+      </c>
+      <c r="K35" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="L34" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="35" s="1" customFormat="1" ht="409.5" spans="1:12">
-      <c r="A35" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G35" s="1" t="s">
+      <c r="L35" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" s="1" customFormat="1" customHeight="1" spans="1:12">
+      <c r="A36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G36" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="H35" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I35" s="1" t="s">
+      <c r="H36" s="1">
+        <v>0</v>
+      </c>
+      <c r="I36" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="J35" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K35" s="1" t="s">
+      <c r="J36" s="1">
+        <v>0</v>
+      </c>
+      <c r="K36" s="1"/>
+      <c r="L36" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" s="1" customFormat="1" customHeight="1" spans="1:12">
+      <c r="A37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G37" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="L35" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="36" s="1" customFormat="1" ht="409.5" spans="1:12">
-      <c r="A36" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G36" s="1" t="s">
+      <c r="H37" s="1">
+        <v>0</v>
+      </c>
+      <c r="I37" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="H36" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I36" s="1" t="s">
+      <c r="J37" s="1">
+        <v>0</v>
+      </c>
+      <c r="K37" s="1"/>
+      <c r="L37" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" s="1" customFormat="1" customHeight="1" spans="1:12">
+      <c r="A38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G38" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="J36" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K36" s="1" t="s">
+      <c r="H38" s="1">
+        <v>0</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K38" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="L36" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="37" s="1" customFormat="1" ht="409.5" spans="1:12">
-      <c r="A37" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G37" s="1" t="s">
+      <c r="L38" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" s="1" customFormat="1" customHeight="1" spans="1:12">
+      <c r="A39" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G39" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="H37" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I37" s="1" t="s">
+      <c r="H39" s="1">
+        <v>0</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K39" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="J37" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K37" s="1" t="s">
+      <c r="L39" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" s="1" customFormat="1" customHeight="1" spans="1:12">
+      <c r="A40" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G40" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="L37" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="38" s="1" customFormat="1" ht="409.5" spans="1:12">
-      <c r="A38" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G38" s="1" t="s">
+      <c r="H40" s="1">
+        <v>0</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K40" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="H38" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I38" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J38" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K38" s="1" t="s">
+      <c r="L40" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" s="1" customFormat="1" customHeight="1" spans="1:12">
+      <c r="A41" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G41" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="L38" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="39" s="1" customFormat="1" ht="409.5" spans="1:12">
-      <c r="A39" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G39" s="1" t="s">
+      <c r="H41" s="1">
+        <v>0</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K41" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="H39" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I39" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J39" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K39" s="1" t="s">
+      <c r="L41" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" s="1" customFormat="1" customHeight="1" spans="1:12">
+      <c r="A42" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K42" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="L39" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="40" s="1" customFormat="1" ht="409.5" spans="1:12">
-      <c r="A40" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G40" s="1" t="s">
+      <c r="L42" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" s="1" customFormat="1" customHeight="1" spans="1:12">
+      <c r="A43" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K43" s="1"/>
+      <c r="L43" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" s="1" customFormat="1" customHeight="1" spans="1:12">
+      <c r="A44" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K44" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="H40" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I40" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J40" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K40" s="1" t="s">
+      <c r="L44" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" s="1" customFormat="1" customHeight="1" spans="1:12">
+      <c r="A45" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J45" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K45" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="L40" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="41" s="1" customFormat="1" ht="409.5" spans="1:12">
-      <c r="A41" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G41" s="1" t="s">
+      <c r="L45" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" s="1" customFormat="1" customHeight="1" spans="1:12">
+      <c r="A46" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J46" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K46" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="H41" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I41" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J41" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K41" s="1" t="s">
+      <c r="L46" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" s="1" customFormat="1" customHeight="1" spans="1:12">
+      <c r="A47" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J47" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K47" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="L41" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="42" s="1" customFormat="1" ht="345.6" spans="1:12">
-      <c r="A42" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H42" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I42" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J42" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K42" s="1" t="s">
+      <c r="L47" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" s="1" customFormat="1" customHeight="1" spans="1:12">
+      <c r="A48" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J48" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K48" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="L42" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="43" s="1" customFormat="1" ht="403.2" spans="1:12">
-      <c r="A43" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H43" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I43" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J43" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K43" s="1" t="s">
+      <c r="L48" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" s="1" customFormat="1" customHeight="1" spans="1:12">
+      <c r="A49" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J49" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K49" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="L43" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="44" s="1" customFormat="1" ht="345.6" spans="1:12">
-      <c r="A44" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G44" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H44" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I44" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J44" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K44" s="1" t="s">
+      <c r="L49" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" s="1" customFormat="1" customHeight="1" spans="1:12">
+      <c r="A50" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J50" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K50" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="L44" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="45" s="1" customFormat="1" ht="331.2" spans="1:12">
-      <c r="A45" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H45" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I45" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J45" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K45" s="1" t="s">
+      <c r="L50" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" s="1" customFormat="1" customHeight="1" spans="1:12">
+      <c r="A51" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J51" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K51" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="L45" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="46" s="1" customFormat="1" ht="409.5" spans="1:12">
-      <c r="A46" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G46" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H46" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I46" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J46" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K46" s="1" t="s">
+      <c r="L51" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" s="1" customFormat="1" customHeight="1" spans="1:12">
+      <c r="A52" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J52" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K52" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="L46" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="47" s="1" customFormat="1" ht="409.5" spans="1:12">
-      <c r="A47" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G47" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H47" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I47" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J47" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K47" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="L47" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="48" s="1" customFormat="1" ht="409.5" spans="1:12">
-      <c r="A48" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G48" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H48" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I48" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J48" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K48" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="L48" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="49" s="1" customFormat="1" ht="374.4" spans="1:12">
-      <c r="A49" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G49" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H49" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I49" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J49" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K49" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="L49" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="50" s="1" customFormat="1" ht="409.5" spans="1:12">
-      <c r="A50" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G50" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H50" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I50" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J50" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K50" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="L50" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="51" s="1" customFormat="1" ht="345.6" spans="1:12">
-      <c r="A51" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G51" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H51" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I51" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J51" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K51" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="L51" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="52" s="1" customFormat="1" ht="409.5" spans="1:12">
-      <c r="A52" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G52" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H52" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I52" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J52" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K52" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="L52" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="53" spans="7:8">
+      <c r="L52" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" customHeight="1" spans="7:12">
       <c r="G53">
         <f>COUNTIF(G2:G52,"*{*")</f>
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H53">
         <f>COUNTIF(H2:H52,"1")</f>
-        <v>2</v>
+        <v>18</v>
+      </c>
+      <c r="I53">
+        <f>COUNTIF(I2:I52,"*{*")</f>
+        <v>14</v>
+      </c>
+      <c r="J53">
+        <f>COUNTIF(J2:J52,"1")</f>
+        <v>8</v>
+      </c>
+      <c r="K53">
+        <f>COUNTIF(K2:K52,"*{*")</f>
+        <v>34</v>
+      </c>
+      <c r="L53">
+        <f>COUNTIF(L2:L52,"1")</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="54" customHeight="1" spans="8:12">
+      <c r="H54">
+        <f>COUNTIF(H2:H52,"0")</f>
+        <v>7</v>
+      </c>
+      <c r="J54">
+        <f>COUNTIF(J2:J52,"0")</f>
+        <v>6</v>
+      </c>
+      <c r="L54">
+        <f>COUNTIF(L2:L52,"0")</f>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>